<commit_message>
Updated the image with score2 being more clear
</commit_message>
<xml_diff>
--- a/Feedbacks/feedback_latest.xlsx
+++ b/Feedbacks/feedback_latest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PY\Bayesian_Framework_Based _Feedback_Scorer_and_Prioritizer\Feedbacks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8A99FC-A217-4CBE-ABE3-2635B8438DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036418B7-9A21-4334-9A15-10632E87A543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>This site does what it’s supposed to, I guess. It’s functional, but nothing special—like plain toast or a cloudy day. I’ve used it a few times without major issues, though it feels a bit slow sometimes. The layout is okay, but honestly, the color scheme is dull and unappealing. Could be better.</t>
+  </si>
+  <si>
+    <t>Breast Cancer</t>
+  </si>
+  <si>
+    <t>Should talk more about male breast though</t>
+  </si>
+  <si>
+    <t>Kidney Cancer</t>
+  </si>
+  <si>
+    <t>WTF is this</t>
   </si>
 </sst>
 </file>
@@ -436,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -448,7 +460,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
@@ -536,6 +548,46 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>697696</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>45638</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>697696</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2">
+        <v>45330</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>